<commit_message>
added insulation cost parameters to input
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input_one_month_one_household_one_car_extreme_2.xlsx
+++ b/src/pv_optimizer_contracting/data_input_one_month_one_household_one_car_extreme_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\OneDrive\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5EBED8-B638-4E5A-BB9F-C2CDA2803A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADB94CC-ADC3-4269-9A7F-A7B1CBC4C794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="10" r:id="rId1"/>
@@ -7525,7 +7525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94768D97-F9DA-444A-B39A-6D1A56841415}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -7870,15 +7870,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952F9C99-337E-41EB-9696-FC2C879F8079}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" customWidth="1"/>
     <col min="5" max="5" width="14.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
   </cols>
@@ -8011,10 +8011,10 @@
         <v>62</v>
       </c>
       <c r="C7">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>5</v>
@@ -8159,11 +8159,11 @@
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <v>0</v>

</xml_diff>